<commit_message>
Limpeza estrutural definitiva do projeto
</commit_message>
<xml_diff>
--- a/excel/PEDIDOS_2026.xlsx
+++ b/excel/PEDIDOS_2026.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USUARIOS\ADM05\Documents\dashboard_tv\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0415BD12-CD0C-4AE1-9BAF-3DF194058D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1B0495-12CD-4521-A63D-CFCF9FC3E79D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{C1828F10-D84A-418A-AAF0-1B51BFAF300A}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" activeTab="1" xr2:uid="{C1828F10-D84A-418A-AAF0-1B51BFAF300A}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -1107,11 +1107,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5695F443-BC3D-48D0-8CD1-D8C4D00277A1}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AU1843"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A183" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B189" sqref="B189"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B192" sqref="B192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1307,7 +1308,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1435,7 +1436,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -1515,7 +1516,7 @@
       <c r="AE3" s="3"/>
       <c r="AK3" s="5"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -1577,7 +1578,7 @@
       <c r="AE4" s="3"/>
       <c r="AK4" s="5"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -1705,7 +1706,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -1785,7 +1786,7 @@
       <c r="AE6" s="3"/>
       <c r="AK6" s="5"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -1845,7 +1846,7 @@
       <c r="AE7" s="3"/>
       <c r="AK7" s="5"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -1970,7 +1971,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -2098,7 +2099,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -2226,7 +2227,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>81</v>
       </c>
@@ -2306,7 +2307,7 @@
       <c r="AE11" s="3"/>
       <c r="AK11" s="5"/>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -2367,7 +2368,7 @@
       <c r="AE12" s="3"/>
       <c r="AK12" s="5"/>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -2442,7 +2443,7 @@
       </c>
       <c r="AK13" s="5"/>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -2501,7 +2502,7 @@
       <c r="AE14" s="3"/>
       <c r="AK14" s="5"/>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -2584,7 +2585,7 @@
       <c r="AE15" s="3"/>
       <c r="AK15" s="5"/>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -2645,7 +2646,7 @@
       <c r="AE16" s="3"/>
       <c r="AK16" s="5"/>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -2725,7 +2726,7 @@
       <c r="AE17" s="3"/>
       <c r="AK17" s="5"/>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -2785,7 +2786,7 @@
       <c r="AE18" s="3"/>
       <c r="AK18" s="5"/>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>96</v>
       </c>
@@ -2913,7 +2914,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -3044,7 +3045,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -3172,7 +3173,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>81</v>
       </c>
@@ -3300,7 +3301,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -3377,7 +3378,7 @@
       <c r="AE23" s="3"/>
       <c r="AK23" s="5"/>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -3434,7 +3435,7 @@
       </c>
       <c r="X24" s="4"/>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -3562,7 +3563,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -3690,7 +3691,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -3821,7 +3822,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -3900,7 +3901,7 @@
       <c r="Z28" s="3"/>
       <c r="AK28" s="5"/>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -3957,7 +3958,7 @@
       </c>
       <c r="X29" s="4"/>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>81</v>
       </c>
@@ -4034,7 +4035,7 @@
       <c r="AE30" s="3"/>
       <c r="AK30" s="5"/>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -4091,7 +4092,7 @@
       </c>
       <c r="X31" s="4"/>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -4216,7 +4217,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -4341,7 +4342,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>96</v>
       </c>
@@ -4472,7 +4473,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>96</v>
       </c>
@@ -4603,7 +4604,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>96</v>
       </c>
@@ -4734,7 +4735,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>96</v>
       </c>
@@ -4865,7 +4866,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>96</v>
       </c>
@@ -4996,7 +4997,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>96</v>
       </c>
@@ -5127,7 +5128,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -5255,7 +5256,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>96</v>
       </c>
@@ -5383,7 +5384,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -5511,7 +5512,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -5639,7 +5640,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -5767,7 +5768,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>96</v>
       </c>
@@ -5848,7 +5849,7 @@
       <c r="AE45" s="3"/>
       <c r="AK45" s="5"/>
     </row>
-    <row r="46" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>63</v>
       </c>
@@ -5912,7 +5913,7 @@
       <c r="AE46" s="3"/>
       <c r="AK46" s="5"/>
     </row>
-    <row r="47" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>96</v>
       </c>
@@ -5991,7 +5992,7 @@
       <c r="AB47" s="3"/>
       <c r="AK47" s="5"/>
     </row>
-    <row r="48" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>63</v>
       </c>
@@ -6052,7 +6053,7 @@
       <c r="X48" s="4"/>
       <c r="AK48" s="5"/>
     </row>
-    <row r="49" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -6132,7 +6133,7 @@
       <c r="AE49" s="3"/>
       <c r="AK49" s="5"/>
     </row>
-    <row r="50" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -6192,7 +6193,7 @@
       <c r="AE50" s="3"/>
       <c r="AK50" s="5"/>
     </row>
-    <row r="51" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>81</v>
       </c>
@@ -6320,7 +6321,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>47</v>
       </c>
@@ -6448,7 +6449,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -6576,7 +6577,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>47</v>
       </c>
@@ -6656,7 +6657,7 @@
       <c r="AE54" s="3"/>
       <c r="AK54" s="5"/>
     </row>
-    <row r="55" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>63</v>
       </c>
@@ -6716,7 +6717,7 @@
       <c r="AE55" s="3"/>
       <c r="AK55" s="5"/>
     </row>
-    <row r="56" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>47</v>
       </c>
@@ -6847,7 +6848,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>136</v>
       </c>
@@ -6927,7 +6928,7 @@
       <c r="AE57" s="3"/>
       <c r="AK57" s="5"/>
     </row>
-    <row r="58" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>63</v>
       </c>
@@ -6988,7 +6989,7 @@
       <c r="X58" s="4"/>
       <c r="AK58" s="5"/>
     </row>
-    <row r="59" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>47</v>
       </c>
@@ -7116,7 +7117,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>81</v>
       </c>
@@ -7244,7 +7245,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>96</v>
       </c>
@@ -7321,7 +7322,7 @@
       <c r="AE61" s="3"/>
       <c r="AK61" s="5"/>
     </row>
-    <row r="62" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>63</v>
       </c>
@@ -7385,7 +7386,7 @@
       <c r="AE62" s="3"/>
       <c r="AK62" s="5"/>
     </row>
-    <row r="63" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>96</v>
       </c>
@@ -7513,7 +7514,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>96</v>
       </c>
@@ -7641,7 +7642,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="65" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>81</v>
       </c>
@@ -7769,7 +7770,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="66" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>81</v>
       </c>
@@ -7897,7 +7898,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>81</v>
       </c>
@@ -8025,7 +8026,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="68" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>81</v>
       </c>
@@ -8153,7 +8154,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="69" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>47</v>
       </c>
@@ -8233,7 +8234,7 @@
       <c r="AE69" s="3"/>
       <c r="AK69" s="5"/>
     </row>
-    <row r="70" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>63</v>
       </c>
@@ -8293,7 +8294,7 @@
       <c r="AE70" s="3"/>
       <c r="AK70" s="5"/>
     </row>
-    <row r="71" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>47</v>
       </c>
@@ -8373,7 +8374,7 @@
       <c r="AE71" s="3"/>
       <c r="AK71" s="5"/>
     </row>
-    <row r="72" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>63</v>
       </c>
@@ -8435,7 +8436,7 @@
       <c r="AB72" s="3"/>
       <c r="AK72" s="5"/>
     </row>
-    <row r="73" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>47</v>
       </c>
@@ -8516,7 +8517,7 @@
       <c r="AE73" s="3"/>
       <c r="AK73" s="5"/>
     </row>
-    <row r="74" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>63</v>
       </c>
@@ -8580,7 +8581,7 @@
       <c r="AE74" s="3"/>
       <c r="AK74" s="5"/>
     </row>
-    <row r="75" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>47</v>
       </c>
@@ -8661,7 +8662,7 @@
       <c r="AE75" s="3"/>
       <c r="AK75" s="5"/>
     </row>
-    <row r="76" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>63</v>
       </c>
@@ -8725,7 +8726,7 @@
       <c r="AE76" s="3"/>
       <c r="AK76" s="5"/>
     </row>
-    <row r="77" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>47</v>
       </c>
@@ -8805,7 +8806,7 @@
       <c r="AE77" s="3"/>
       <c r="AK77" s="5"/>
     </row>
-    <row r="78" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>63</v>
       </c>
@@ -8868,7 +8869,7 @@
       <c r="AE78" s="3"/>
       <c r="AK78" s="5"/>
     </row>
-    <row r="79" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>96</v>
       </c>
@@ -8946,7 +8947,7 @@
       <c r="AE79" s="3"/>
       <c r="AK79" s="5"/>
     </row>
-    <row r="80" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>63</v>
       </c>
@@ -9010,7 +9011,7 @@
       <c r="AE80" s="3"/>
       <c r="AK80" s="5"/>
     </row>
-    <row r="81" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>96</v>
       </c>
@@ -9088,7 +9089,7 @@
       <c r="AE81" s="3"/>
       <c r="AK81" s="5"/>
     </row>
-    <row r="82" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>63</v>
       </c>
@@ -9153,7 +9154,7 @@
       <c r="AE82" s="3"/>
       <c r="AK82" s="5"/>
     </row>
-    <row r="83" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>47</v>
       </c>
@@ -9281,7 +9282,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="84" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>47</v>
       </c>
@@ -9409,7 +9410,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="85" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>47</v>
       </c>
@@ -9490,7 +9491,7 @@
       <c r="AE85" s="3"/>
       <c r="AK85" s="5"/>
     </row>
-    <row r="86" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>63</v>
       </c>
@@ -9548,7 +9549,7 @@
       <c r="X86" s="4"/>
       <c r="AK86" s="5"/>
     </row>
-    <row r="87" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>96</v>
       </c>
@@ -9676,7 +9677,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="88" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>96</v>
       </c>
@@ -9804,7 +9805,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="89" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>47</v>
       </c>
@@ -9935,7 +9936,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="90" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>47</v>
       </c>
@@ -10015,7 +10016,7 @@
       <c r="AE90" s="3"/>
       <c r="AK90" s="5"/>
     </row>
-    <row r="91" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>63</v>
       </c>
@@ -10078,7 +10079,7 @@
       <c r="AE91" s="3"/>
       <c r="AK91" s="5"/>
     </row>
-    <row r="92" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>96</v>
       </c>
@@ -10159,7 +10160,7 @@
       <c r="AE92" s="3"/>
       <c r="AK92" s="5"/>
     </row>
-    <row r="93" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>63</v>
       </c>
@@ -10222,7 +10223,7 @@
       <c r="AE93" s="3"/>
       <c r="AK93" s="5"/>
     </row>
-    <row r="94" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>96</v>
       </c>
@@ -10350,7 +10351,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="95" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>47</v>
       </c>
@@ -10430,7 +10431,7 @@
       <c r="AE95" s="3"/>
       <c r="AK95" s="5"/>
     </row>
-    <row r="96" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>63</v>
       </c>
@@ -10495,7 +10496,7 @@
       <c r="AE96" s="3"/>
       <c r="AK96" s="5"/>
     </row>
-    <row r="97" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>47</v>
       </c>
@@ -10620,7 +10621,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="98" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>47</v>
       </c>
@@ -10745,7 +10746,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="99" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>81</v>
       </c>
@@ -10873,7 +10874,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="100" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>47</v>
       </c>
@@ -11004,7 +11005,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="101" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>96</v>
       </c>
@@ -11135,7 +11136,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="102" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>96</v>
       </c>
@@ -11263,7 +11264,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="103" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>47</v>
       </c>
@@ -11344,7 +11345,7 @@
       <c r="AE103" s="3"/>
       <c r="AK103" s="5"/>
     </row>
-    <row r="104" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>63</v>
       </c>
@@ -11406,7 +11407,7 @@
       <c r="AE104" s="3"/>
       <c r="AK104" s="5"/>
     </row>
-    <row r="105" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>47</v>
       </c>
@@ -11531,7 +11532,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="106" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>47</v>
       </c>
@@ -11656,7 +11657,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="107" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>47</v>
       </c>
@@ -11736,7 +11737,7 @@
       <c r="AE107" s="3"/>
       <c r="AK107" s="5"/>
     </row>
-    <row r="108" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>63</v>
       </c>
@@ -11796,7 +11797,7 @@
       <c r="AE108" s="3"/>
       <c r="AK108" s="5"/>
     </row>
-    <row r="109" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>96</v>
       </c>
@@ -11924,7 +11925,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="110" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>96</v>
       </c>
@@ -12052,7 +12053,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="111" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>47</v>
       </c>
@@ -12183,7 +12184,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="112" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>47</v>
       </c>
@@ -12265,7 +12266,7 @@
       <c r="AE112" s="3"/>
       <c r="AK112" s="5"/>
     </row>
-    <row r="113" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>63</v>
       </c>
@@ -12329,7 +12330,7 @@
       <c r="AE113" s="3"/>
       <c r="AK113" s="5"/>
     </row>
-    <row r="114" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>96</v>
       </c>
@@ -12406,7 +12407,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="115" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>63</v>
       </c>
@@ -12464,7 +12465,7 @@
       <c r="X115" s="4"/>
       <c r="AK115" s="5"/>
     </row>
-    <row r="116" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>96</v>
       </c>
@@ -12595,7 +12596,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="117" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>96</v>
       </c>
@@ -12675,7 +12676,7 @@
       <c r="AE117" s="3"/>
       <c r="AK117" s="5"/>
     </row>
-    <row r="118" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>63</v>
       </c>
@@ -12739,7 +12740,7 @@
       <c r="AE118" s="3"/>
       <c r="AK118" s="5"/>
     </row>
-    <row r="119" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>96</v>
       </c>
@@ -12820,7 +12821,7 @@
       <c r="AE119" s="3"/>
       <c r="AK119" s="5"/>
     </row>
-    <row r="120" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>63</v>
       </c>
@@ -12884,7 +12885,7 @@
       <c r="AE120" s="3"/>
       <c r="AK120" s="5"/>
     </row>
-    <row r="121" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>47</v>
       </c>
@@ -12965,7 +12966,7 @@
       <c r="AE121" s="3"/>
       <c r="AK121" s="5"/>
     </row>
-    <row r="122" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>63</v>
       </c>
@@ -13026,7 +13027,7 @@
       <c r="AE122" s="3"/>
       <c r="AK122" s="5"/>
     </row>
-    <row r="123" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>47</v>
       </c>
@@ -13154,7 +13155,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="124" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>96</v>
       </c>
@@ -13285,7 +13286,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="125" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>96</v>
       </c>
@@ -13365,7 +13366,7 @@
       <c r="AE125" s="3"/>
       <c r="AK125" s="5"/>
     </row>
-    <row r="126" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>63</v>
       </c>
@@ -13425,7 +13426,7 @@
       <c r="AE126" s="3"/>
       <c r="AK126" s="5"/>
     </row>
-    <row r="127" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>47</v>
       </c>
@@ -13505,7 +13506,7 @@
       <c r="AE127" s="3"/>
       <c r="AK127" s="5"/>
     </row>
-    <row r="128" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>63</v>
       </c>
@@ -13566,7 +13567,7 @@
       <c r="AE128" s="3"/>
       <c r="AK128" s="5"/>
     </row>
-    <row r="129" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>96</v>
       </c>
@@ -13694,7 +13695,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="130" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>47</v>
       </c>
@@ -13771,7 +13772,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="131" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>63</v>
       </c>
@@ -13827,7 +13828,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="132" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>81</v>
       </c>
@@ -13904,7 +13905,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="133" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>63</v>
       </c>
@@ -13960,7 +13961,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="134" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>47</v>
       </c>
@@ -14038,7 +14039,7 @@
       </c>
       <c r="AK134" s="5"/>
     </row>
-    <row r="135" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>63</v>
       </c>
@@ -14101,7 +14102,7 @@
       <c r="AE135" s="3"/>
       <c r="AK135" s="5"/>
     </row>
-    <row r="136" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>47</v>
       </c>
@@ -14229,7 +14230,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="137" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>47</v>
       </c>
@@ -14354,7 +14355,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="138" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>47</v>
       </c>
@@ -14482,7 +14483,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="139" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>81</v>
       </c>
@@ -14560,7 +14561,7 @@
       <c r="AE139" s="3"/>
       <c r="AK139" s="5"/>
     </row>
-    <row r="140" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>63</v>
       </c>
@@ -15087,7 +15088,7 @@
       <c r="AE144" s="3"/>
       <c r="AK144" s="5"/>
     </row>
-    <row r="145" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>63</v>
       </c>
@@ -15228,7 +15229,7 @@
       <c r="AE146" s="3"/>
       <c r="AK146" s="5"/>
     </row>
-    <row r="147" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>63</v>
       </c>
@@ -15368,7 +15369,7 @@
       <c r="AE148" s="3"/>
       <c r="AK148" s="5"/>
     </row>
-    <row r="149" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>63</v>
       </c>
@@ -15509,7 +15510,7 @@
       <c r="AE150" s="3"/>
       <c r="AK150" s="5"/>
     </row>
-    <row r="151" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>63</v>
       </c>
@@ -15776,7 +15777,7 @@
       <c r="AE153" s="3"/>
       <c r="AK153" s="5"/>
     </row>
-    <row r="154" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>63</v>
       </c>
@@ -15916,7 +15917,7 @@
       <c r="AE155" s="3"/>
       <c r="AK155" s="5"/>
     </row>
-    <row r="156" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>63</v>
       </c>
@@ -16952,7 +16953,7 @@
       <c r="AE164" s="3"/>
       <c r="AK164" s="5"/>
     </row>
-    <row r="165" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>63</v>
       </c>
@@ -17482,7 +17483,7 @@
       <c r="AE169" s="3"/>
       <c r="AK169" s="5"/>
     </row>
-    <row r="170" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>63</v>
       </c>
@@ -17621,7 +17622,7 @@
       <c r="AB171" s="3"/>
       <c r="AK171" s="5"/>
     </row>
-    <row r="172" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>63</v>
       </c>
@@ -17757,7 +17758,7 @@
       <c r="AB173" s="3"/>
       <c r="AK173" s="5"/>
     </row>
-    <row r="174" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>63</v>
       </c>
@@ -17897,7 +17898,7 @@
       <c r="AB175" s="3"/>
       <c r="AK175" s="5"/>
     </row>
-    <row r="176" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>63</v>
       </c>
@@ -18031,7 +18032,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="178" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>63</v>
       </c>
@@ -19193,7 +19194,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="188" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>63</v>
       </c>
@@ -19712,7 +19713,7 @@
       <c r="AE192" s="3"/>
       <c r="AK192" s="5"/>
     </row>
-    <row r="193" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>63</v>
       </c>
@@ -20227,7 +20228,7 @@
       <c r="AE197" s="3"/>
       <c r="AK197" s="5"/>
     </row>
-    <row r="198" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>63</v>
       </c>
@@ -20492,7 +20493,7 @@
       <c r="AB200" s="3"/>
       <c r="AK200" s="5"/>
     </row>
-    <row r="201" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>63</v>
       </c>
@@ -20630,7 +20631,7 @@
       <c r="AE202" s="3"/>
       <c r="AK202" s="5"/>
     </row>
-    <row r="203" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>63</v>
       </c>
@@ -20766,7 +20767,7 @@
       </c>
       <c r="AK204" s="5"/>
     </row>
-    <row r="205" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>63</v>
       </c>
@@ -20904,7 +20905,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="207" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>63</v>
       </c>
@@ -21046,7 +21047,7 @@
       <c r="AE208" s="3"/>
       <c r="AK208" s="5"/>
     </row>
-    <row r="209" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>63</v>
       </c>
@@ -21190,7 +21191,7 @@
       <c r="AE210" s="3"/>
       <c r="AK210" s="5"/>
     </row>
-    <row r="211" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>63</v>
       </c>
@@ -21333,7 +21334,7 @@
       <c r="AE212" s="3"/>
       <c r="AK212" s="5"/>
     </row>
-    <row r="213" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>63</v>
       </c>
@@ -21476,7 +21477,7 @@
       <c r="AE214" s="3"/>
       <c r="AK214" s="5"/>
     </row>
-    <row r="215" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>63</v>
       </c>
@@ -40348,7 +40349,13 @@
       <c r="H1843" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AU215" xr:uid="{5695F443-BC3D-48D0-8CD1-D8C4D00277A1}"/>
+  <autoFilter ref="A1:AU215" xr:uid="{5695F443-BC3D-48D0-8CD1-D8C4D00277A1}">
+    <filterColumn colId="4">
+      <filters>
+        <dateGroupItem year="2026" month="2" dateTimeGrouping="month"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="B1:B1823 B1825:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
@@ -40361,8 +40368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3563FB9-48F3-41D1-B6BA-29C9EE90DA6F}">
   <dimension ref="A2:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -40378,7 +40385,7 @@
         <v>2026</v>
       </c>
       <c r="D2">
-        <v>2026</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -40387,13 +40394,13 @@
       </c>
       <c r="B3" s="11">
         <f>SUBTOTAL(9,Planilha1!K1:K1825)</f>
-        <v>1903431.87</v>
+        <v>597360.66999999981</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="11">
-        <v>442403.79999999987</v>
+        <v>602596.14999999991</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -40402,13 +40409,13 @@
       </c>
       <c r="B4" s="9">
         <f>SUBTOTAL(9,Planilha1!L1:L1820)</f>
-        <v>313431.23000000004</v>
+        <v>103873.66</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="9">
-        <v>83459.710000000006</v>
+        <v>89741.94</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -40417,13 +40424,13 @@
       </c>
       <c r="B5" s="12">
         <f>SUBTOTAL(9,Planilha1!M1:M1821)</f>
-        <v>3003571.5794212953</v>
+        <v>46907.729999999996</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="12">
-        <v>33872.180000000008</v>
+        <v>44216.9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -40432,13 +40439,13 @@
       </c>
       <c r="B6" s="10">
         <f>SUBTOTAL(3,Planilha1!D2:D1821)</f>
-        <v>214</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
         <v>214</v>
       </c>
       <c r="E6" s="10">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -40447,13 +40454,13 @@
       </c>
       <c r="B7" s="13">
         <f>B3/B6</f>
-        <v>8894.541448598131</v>
+        <v>11487.705192307689</v>
       </c>
       <c r="D7" t="s">
         <v>217</v>
       </c>
       <c r="E7" s="13">
-        <v>9412.846808510636</v>
+        <v>11815.610784313723</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -40462,13 +40469,13 @@
       </c>
       <c r="B8" s="13">
         <f>B3/B4</f>
-        <v>6.0728851748436172</v>
+        <v>5.7508387593158821</v>
       </c>
       <c r="D8" t="s">
         <v>216</v>
       </c>
       <c r="E8" s="13">
-        <v>5.3008068204406635</v>
+        <v>6.714766250874451</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -40477,13 +40484,13 @@
       </c>
       <c r="B9" s="13">
         <f>B3/B5</f>
-        <v>0.63372282619838161</v>
+        <v>12.734802344943997</v>
       </c>
       <c r="D9" t="s">
         <v>215</v>
       </c>
       <c r="E9" s="13">
-        <v>13.060978065185051</v>
+        <v>13.628186281715813</v>
       </c>
     </row>
   </sheetData>

</xml_diff>